<commit_message>
Comitting all files to Git Local Repository
</commit_message>
<xml_diff>
--- a/Test1.xlsx
+++ b/Test1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Interview Preparation\Git_GitHub Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C1F9B7-B9A8-4374-A1AE-298029A8300E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0EBF60-4CC7-4522-896C-406CFBA96E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34830" yWindow="6000" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Dinesh</t>
+  </si>
+  <si>
+    <t>Mundhe</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -337,90 +348,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A50"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>

</xml_diff>